<commit_message>
fixing wrong sum with NA
</commit_message>
<xml_diff>
--- a/input/SSA_questionnaire.xlsx
+++ b/input/SSA_questionnaire.xlsx
@@ -63503,8 +63503,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE51FB2AFBB2DD429D3D11FE759FFC43" ma:contentTypeVersion="18" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="df5b28ce25a628da7e4351ecd50f592e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f4877444-78fa-4cfa-bafc-d6c64fafc061" xmlns:ns3="d0fa6634-326e-4532-91a2-52bea7ac9212" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="829ade136f372bbc1f9334b9c4b8c0cd" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE51FB2AFBB2DD429D3D11FE759FFC43" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64bf7a86c00e57391fde19f51239d445">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f4877444-78fa-4cfa-bafc-d6c64fafc061" xmlns:ns3="d0fa6634-326e-4532-91a2-52bea7ac9212" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="887bdea85c641648dfa41b2556fd8924" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
     <xsd:import namespace="d0fa6634-326e-4532-91a2-52bea7ac9212"/>
@@ -63541,12 +63541,12 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="24" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="24" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="25" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="25" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -63590,7 +63590,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="18" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="4d06f0b5-5743-41f2-90d3-b12c8ffc7f36" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="18" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="4d06f0b5-5743-41f2-90d3-b12c8ffc7f36" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -63623,7 +63623,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d0fa6634-326e-4532-91a2-52bea7ac9212" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -63642,7 +63642,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -63670,8 +63670,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -63781,5 +63781,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2005541-FA1A-403E-B399-C1F6F8793D94}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33DF0D7B-5664-4C73-B75F-7DF7CCEFBC70}"/>
 </file>
</xml_diff>